<commit_message>
Updated optimizer from bayesopt to random search - updated experiment and results of Lx parameter with new optimizer
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Lx_Parameters_Estimation/1-Trained-Models/Trained-All-Dataset-k-5/Results-Trained-model-k-5.xlsx
+++ b/Parameters-Estimation/Lx_Parameters_Estimation/1-Trained-Models/Trained-All-Dataset-k-5/Results-Trained-model-k-5.xlsx
@@ -13,7 +13,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>random_forest</t>
+  </si>
+  <si>
+    <t>lsboost</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>NRMSE</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>RSE</t>
+  </si>
+  <si>
+    <t>RRSE</t>
+  </si>
+  <si>
+    <t>RAE</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Corr Coeff</t>
+  </si>
   <si>
     <t>Row</t>
   </si>
@@ -100,96 +133,96 @@
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
     <col min="5" max="5" width="12.7109375" customWidth="true"/>
     <col min="6" max="6" width="12.7109375" customWidth="true"/>
-    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
     <col min="8" max="8" width="12.7109375" customWidth="true"/>
     <col min="9" max="9" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0">
-        <v>3.9440234160163832</v>
+        <v>1.9917072969183665</v>
       </c>
       <c r="C2" s="0">
-        <v>0.32514620082575291</v>
+        <v>0.17949777369487804</v>
       </c>
       <c r="D2" s="0">
-        <v>3.3395583213083215</v>
+        <v>1.5555997234247234</v>
       </c>
       <c r="E2" s="0">
-        <v>0.34497285972469732</v>
+        <v>0.32711871149002608</v>
       </c>
       <c r="F2" s="0">
-        <v>0.58734390243255041</v>
+        <v>0.57194292677681235</v>
       </c>
       <c r="G2" s="0">
-        <v>0.66094966116406939</v>
+        <v>0.60328234496180966</v>
       </c>
       <c r="H2" s="0">
-        <v>0.65502714027530273</v>
+        <v>0.67288128850997397</v>
       </c>
       <c r="I2" s="0">
-        <v>0.81424446238608261</v>
+        <v>0.85328615764239202</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0">
-        <v>3.8781885608050928</v>
+        <v>1.0819613690389691</v>
       </c>
       <c r="C3" s="0">
-        <v>0.31971876016530026</v>
+        <v>0.097509135637974878</v>
       </c>
       <c r="D3" s="0">
-        <v>3.0812996264946064</v>
+        <v>0.8523946312535684</v>
       </c>
       <c r="E3" s="0">
-        <v>0.33355219387184731</v>
+        <v>0.096533458837287769</v>
       </c>
       <c r="F3" s="0">
-        <v>0.57753977687415381</v>
+        <v>0.31069834057697793</v>
       </c>
       <c r="G3" s="0">
-        <v>0.60983631610264011</v>
+        <v>0.33057002018706899</v>
       </c>
       <c r="H3" s="0">
-        <v>0.66644780612815269</v>
+        <v>0.90346654116271219</v>
       </c>
       <c r="I3" s="0">
-        <v>0.8172207763768542</v>
+        <v>0.95286773584691631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>